<commit_message>
Update with more input validation and better logging
</commit_message>
<xml_diff>
--- a/relays-creator/examples/excel.xlsx
+++ b/relays-creator/examples/excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenezia/biot-tools/relays-creator/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenezia/biot-tools/relays-creator/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBBAFA0-9B74-8244-AEE1-255D8B3D3576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C3B5F4-52CE-8E46-8DBC-B60A026E4C3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="27640" windowHeight="15640" xr2:uid="{345AA04F-B42B-5143-968F-05FF6E902C33}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add support for updates as well
</commit_message>
<xml_diff>
--- a/relays-creator/examples/excel.xlsx
+++ b/relays-creator/examples/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenezia/biot-tools/relays-creator/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C3B5F4-52CE-8E46-8DBC-B60A026E4C3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A55F80-C2A4-EC41-A0D7-030EC8C75F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="27640" windowHeight="15640" xr2:uid="{345AA04F-B42B-5143-968F-05FF6E902C33}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Case Serial Number</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>script2</t>
+  </si>
+  <si>
+    <t>relay_100</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,9 +542,8 @@
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="4" t="str">
-        <f>"Relay_"&amp;A2</f>
-        <v>Relay_script1</v>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>9</v>

</xml_diff>